<commit_message>
Jan 17 - report
</commit_message>
<xml_diff>
--- a/graph/Jan 17/Report.xlsx
+++ b/graph/Jan 17/Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="14900" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="31140" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Morning</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Average</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Peter Kok - Best</t>
+  </si>
+  <si>
+    <t>Peter Kok - Average</t>
+  </si>
+  <si>
+    <t>Zainuddin - Best</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -44,9 +59,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,13 +84,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -96,18 +151,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,15 +505,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
@@ -806,28 +875,113 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="2">
+      <c r="A23" s="6">
         <f>AVERAGE(A2:A21)</f>
         <v>1.119402551182604</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="6">
         <f t="shared" ref="B23:E23" si="0">AVERAGE(B2:B21)</f>
         <v>2.1346739610020697</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="6">
         <f t="shared" si="0"/>
         <v>0.99929955007426741</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="6">
         <f t="shared" si="0"/>
         <v>0.79552471312584394</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>1.883763092201995</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="7" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="8">
+        <f>A2</f>
+        <v>0.42581314658488001</v>
+      </c>
+      <c r="B24" s="8">
+        <f t="shared" ref="B24:E24" si="1">B2</f>
+        <v>1.3205461789841</v>
+      </c>
+      <c r="C24" s="8">
+        <f t="shared" si="1"/>
+        <v>0.57947712640284998</v>
+      </c>
+      <c r="D24" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40365118466109001</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="1"/>
+        <v>1.4211104679269</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="C26" s="7">
+        <v>2.4</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2.1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B29" s="5">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="C29" s="5">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -835,6 +989,7 @@
     <sortCondition ref="E2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>